<commit_message>
cập nhật file mẫu
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Certificate-Request-Infomation.xlsx
+++ b/src/main/resources/templates/excel/Certificate-Request-Infomation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CRM\webapp\public\invoiceform\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
   </bookViews>
   <sheets>
     <sheet name="Dữ liệu đầu vào CTS" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
+    <author>Admin</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0">
@@ -215,7 +216,9 @@
 - CTS Cá nhân
 Không dành cho:
 - CTS Doanh nghiệp
-Tình trạng: Bắt buộc</t>
+Tình trạng: Bắt buộc
+Bắt đầu bằng ký tự '
+</t>
         </r>
       </text>
     </comment>
@@ -300,7 +303,9 @@
           <t xml:space="preserve">
 Trường này dành cho:
 - Tất cả loại CTS
-Tình trạng: Không bắt buộc</t>
+Tình trạng: Không bắt buộc
+- Bắt đầu bằng ký tự '
+</t>
         </r>
       </text>
     </comment>
@@ -513,6 +518,162 @@
           </rPr>
           <t xml:space="preserve">
 Dữ liệu được hệ thống EasySign sinh ra sau khi import CTS thành công - Người dùng không nhập vào cột này</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thông tin bắt buộc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thông tin bắt buộc</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Thông tin bắt buộc
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Thông tin bắt buộc
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thông tin bắt buộc</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thông tin bắt buộc</t>
         </r>
       </text>
     </comment>
@@ -926,7 +1087,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -998,6 +1159,26 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1133,7 +1314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1210,8 +1391,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1501,10 +1680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1595,10 +1774,10 @@
       <c r="S1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="T1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="U1" s="27" t="s">
         <v>19</v>
       </c>
       <c r="V1" s="8" t="s">
@@ -1678,8 +1857,8 @@
       <c r="S2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="28"/>
-      <c r="U2" s="30"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="28"/>
       <c r="V2" s="18" t="s">
         <v>41</v>
       </c>
@@ -1698,14 +1877,6 @@
       <c r="AA2" s="10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="G3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="W3" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>